<commit_message>
Correcciones de memoria EEPROM ATMEGA
Se modificó el código de la escritura de la memoria EEPROM en el ATMEGA para realizar una comparación más justa con el PIC. Los resultados obtenidos se guardaron en los archivos .sal correspondientes a "ATMEGAajustado" en el compilado de datos de la memoria EEPROM.
</commit_message>
<xml_diff>
--- a/Analisis/Temporizador/TemporizadorSinInterrupcionesASM.xlsx
+++ b/Analisis/Temporizador/TemporizadorSinInterrupcionesASM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schinzii\Desktop\UVG\Semestre 10\Design 2\AVR_vs_PIC\Analisis\Temporizador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8EE6E7-FA6F-47F6-9F1F-22DD9CF273EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7871F1DD-A2DE-45BC-B287-D4845263F130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{1CDCDDEF-6B39-4217-A858-53EB810ACCBE}"/>
   </bookViews>
@@ -18253,7 +18253,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="2038350" y="3048000"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:ext cx="4629150" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -18368,7 +18368,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8953500" y="3048000"/>
+              <a:off x="9115425" y="3048000"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -49294,8 +49294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95059EC-D0AC-49A5-9AD2-A5FCAE21BF60}">
   <dimension ref="A1:S1207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q35" sqref="Q35"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33:S34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49304,7 +49304,7 @@
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>